<commit_message>
Added some testing capabilities
Completion tolerance and finishing time can now be set the restrictions
sheet
</commit_message>
<xml_diff>
--- a/input_BSZ2030.xlsx
+++ b/input_BSZ2030.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" tabRatio="912" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" tabRatio="912" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -319,7 +319,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1979" uniqueCount="896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2022" uniqueCount="909">
   <si>
     <t>Name</t>
   </si>
@@ -3006,7 +3006,46 @@
     <t>PtF-DME</t>
   </si>
   <si>
-    <t>UNKNOWN</t>
+    <t>1-bm_MeOH</t>
+  </si>
+  <si>
+    <t>BM-MeOh</t>
+  </si>
+  <si>
+    <t>1-bm_dme</t>
+  </si>
+  <si>
+    <t>1-h2_MeOH</t>
+  </si>
+  <si>
+    <t>1-h2_DME</t>
+  </si>
+  <si>
+    <t>2-bm_MeOH</t>
+  </si>
+  <si>
+    <t>2-h2_MeOH</t>
+  </si>
+  <si>
+    <t>2-h2_DME</t>
+  </si>
+  <si>
+    <t>1-EC_5</t>
+  </si>
+  <si>
+    <t>1-EC_6</t>
+  </si>
+  <si>
+    <t>2-bm_DME</t>
+  </si>
+  <si>
+    <t>MIPGap</t>
+  </si>
+  <si>
+    <t>TimeLimit</t>
+  </si>
+  <si>
+    <t>ImproveStartTime</t>
   </si>
 </sst>
 </file>
@@ -3940,8 +3979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4395,7 +4434,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="38" t="s">
-        <v>895</v>
+        <v>888</v>
       </c>
       <c r="J8" s="43">
         <v>0</v>
@@ -4448,7 +4487,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="38" t="s">
-        <v>895</v>
+        <v>888</v>
       </c>
       <c r="J9" s="43">
         <v>0</v>
@@ -4743,7 +4782,7 @@
         <v>6.8844221105527653E-2</v>
       </c>
       <c r="I14" s="46" t="s">
-        <v>895</v>
+        <v>890</v>
       </c>
       <c r="J14" s="51">
         <v>0</v>
@@ -4801,7 +4840,7 @@
         <v>6.6920943134535366E-2</v>
       </c>
       <c r="I15" s="46" t="s">
-        <v>895</v>
+        <v>890</v>
       </c>
       <c r="J15" s="51">
         <v>0</v>
@@ -5400,10 +5439,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5511,43 +5550,43 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
-        <v>837</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>833</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>7</v>
+    <row r="8" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
+        <v>895</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>896</v>
+      </c>
+      <c r="D8" s="52" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="52" t="s">
+        <v>897</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>892</v>
+      </c>
+      <c r="D9" s="52" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
-        <v>838</v>
+        <v>34</v>
       </c>
       <c r="B10" s="32" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>834</v>
+        <v>11</v>
       </c>
       <c r="D10" s="32" t="s">
         <v>7</v>
@@ -5555,13 +5594,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
-        <v>871</v>
+        <v>837</v>
       </c>
       <c r="B11" s="32" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>863</v>
+        <v>833</v>
       </c>
       <c r="D11" s="32" t="s">
         <v>7</v>
@@ -5569,150 +5608,150 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>829</v>
+        <v>6</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>11</v>
+        <v>834</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>830</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
-        <v>840</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>829</v>
+        <v>871</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>6</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>833</v>
+        <v>863</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
-        <v>841</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>829</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>834</v>
-      </c>
-      <c r="D14" s="32" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
-        <v>886</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>829</v>
-      </c>
-      <c r="C15" s="33" t="s">
-        <v>863</v>
-      </c>
-      <c r="D15" s="33" t="s">
-        <v>830</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="52" t="s">
+        <v>898</v>
+      </c>
+      <c r="B14" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="52" t="s">
+        <v>893</v>
+      </c>
+      <c r="D14" s="52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="52" t="s">
+        <v>899</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="52" t="s">
+        <v>894</v>
+      </c>
+      <c r="D15" s="52" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>9</v>
+        <v>829</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>8</v>
+        <v>830</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
-        <v>843</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>9</v>
+        <v>840</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>829</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>36</v>
+        <v>833</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>29</v>
+        <v>830</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
-        <v>844</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>9</v>
+        <v>841</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>829</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>845</v>
+        <v>834</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
-        <v>846</v>
-      </c>
-      <c r="B19" s="32" t="s">
-        <v>832</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
-        <v>847</v>
-      </c>
-      <c r="B20" s="32" t="s">
-        <v>832</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
-        <v>872</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>860</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>873</v>
-      </c>
-      <c r="D21" s="32" t="s">
-        <v>861</v>
+        <v>830</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>886</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>829</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>863</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="52" t="s">
+        <v>903</v>
+      </c>
+      <c r="B20" s="52" t="s">
+        <v>829</v>
+      </c>
+      <c r="C20" s="52" t="s">
+        <v>893</v>
+      </c>
+      <c r="D20" s="52" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="52" t="s">
+        <v>904</v>
+      </c>
+      <c r="B21" s="52" t="s">
+        <v>829</v>
+      </c>
+      <c r="C21" s="52" t="s">
+        <v>894</v>
+      </c>
+      <c r="D21" s="52" t="s">
+        <v>830</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
-        <v>37</v>
+        <v>842</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="C22" s="32" t="s">
         <v>35</v>
@@ -5723,10 +5762,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
-        <v>38</v>
+        <v>843</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C23" s="32" t="s">
         <v>36</v>
@@ -5737,24 +5776,24 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
-        <v>874</v>
+        <v>844</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>862</v>
+        <v>9</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>873</v>
+        <v>845</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>861</v>
+        <v>831</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
-        <v>39</v>
+        <v>846</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>11</v>
+        <v>832</v>
       </c>
       <c r="C25" s="32" t="s">
         <v>35</v>
@@ -5765,38 +5804,38 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
-        <v>849</v>
+        <v>872</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>833</v>
+        <v>860</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>36</v>
+        <v>873</v>
       </c>
       <c r="D27" s="32" t="s">
-        <v>29</v>
+        <v>861</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="32" t="s">
-        <v>850</v>
+        <v>37</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>834</v>
+        <v>30</v>
       </c>
       <c r="C28" s="32" t="s">
         <v>35</v>
@@ -5807,10 +5846,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
-        <v>851</v>
+        <v>38</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>834</v>
+        <v>31</v>
       </c>
       <c r="C29" s="32" t="s">
         <v>36</v>
@@ -5821,83 +5860,83 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
-        <v>852</v>
+        <v>874</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>834</v>
+        <v>862</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>845</v>
+        <v>873</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
-        <v>875</v>
-      </c>
-      <c r="B31" s="32" t="s">
-        <v>863</v>
-      </c>
-      <c r="C31" s="32" t="s">
-        <v>873</v>
-      </c>
-      <c r="D31" s="32" t="s">
         <v>861</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" s="32" t="s">
+    <row r="31" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="52" t="s">
+        <v>900</v>
+      </c>
+      <c r="B31" s="52" t="s">
+        <v>891</v>
+      </c>
+      <c r="C31" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="32" t="s">
+      <c r="D31" s="52" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="52" t="s">
+        <v>905</v>
+      </c>
+      <c r="B32" s="52" t="s">
+        <v>892</v>
+      </c>
+      <c r="C32" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="52" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="32" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B33" s="32" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="32" t="s">
-        <v>876</v>
+        <v>848</v>
       </c>
       <c r="B34" s="32" t="s">
-        <v>873</v>
+        <v>833</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>864</v>
+        <v>35</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>861</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="32" t="s">
-        <v>46</v>
+        <v>849</v>
       </c>
       <c r="B35" s="32" t="s">
+        <v>833</v>
+      </c>
+      <c r="C35" s="32" t="s">
         <v>36</v>
-      </c>
-      <c r="C35" s="32" t="s">
-        <v>44</v>
       </c>
       <c r="D35" s="32" t="s">
         <v>29</v>
@@ -5905,27 +5944,27 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
-        <v>47</v>
+        <v>850</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>36</v>
+        <v>834</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="32" t="s">
-        <v>60</v>
+        <v>851</v>
       </c>
       <c r="B37" s="32" t="s">
+        <v>834</v>
+      </c>
+      <c r="C37" s="32" t="s">
         <v>36</v>
-      </c>
-      <c r="C37" s="32" t="s">
-        <v>58</v>
       </c>
       <c r="D37" s="32" t="s">
         <v>29</v>
@@ -5933,239 +5972,379 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="32" t="s">
-        <v>61</v>
+        <v>852</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>36</v>
+        <v>834</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>59</v>
+        <v>845</v>
       </c>
       <c r="D38" s="32" t="s">
-        <v>29</v>
+        <v>831</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="32" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="B39" s="32" t="s">
+        <v>863</v>
+      </c>
+      <c r="C39" s="32" t="s">
         <v>873</v>
-      </c>
-      <c r="C39" s="32" t="s">
-        <v>865</v>
       </c>
       <c r="D39" s="32" t="s">
         <v>861</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="32" t="s">
-        <v>878</v>
-      </c>
-      <c r="B40" s="32" t="s">
-        <v>873</v>
-      </c>
-      <c r="C40" s="32" t="s">
-        <v>866</v>
-      </c>
-      <c r="D40" s="32" t="s">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="32" t="s">
-        <v>879</v>
-      </c>
-      <c r="B41" s="32" t="s">
-        <v>873</v>
-      </c>
-      <c r="C41" s="32" t="s">
-        <v>867</v>
-      </c>
-      <c r="D41" s="32" t="s">
-        <v>861</v>
+    <row r="40" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="52" t="s">
+        <v>901</v>
+      </c>
+      <c r="B40" s="52" t="s">
+        <v>893</v>
+      </c>
+      <c r="C40" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="52" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="52" t="s">
+        <v>902</v>
+      </c>
+      <c r="B41" s="52" t="s">
+        <v>894</v>
+      </c>
+      <c r="C41" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="52" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="32" t="s">
-        <v>880</v>
+        <v>40</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>873</v>
+        <v>35</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>868</v>
+        <v>50</v>
       </c>
       <c r="D42" s="32" t="s">
-        <v>861</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="32" t="s">
-        <v>853</v>
+        <v>52</v>
       </c>
       <c r="B43" s="32" t="s">
-        <v>845</v>
+        <v>36</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>831</v>
+        <v>51</v>
       </c>
       <c r="D43" s="32" t="s">
-        <v>831</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="32" t="s">
-        <v>41</v>
+        <v>876</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>50</v>
+        <v>873</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>27</v>
+        <v>864</v>
       </c>
       <c r="D44" s="32" t="s">
-        <v>27</v>
+        <v>861</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="32" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D45" s="32" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
-        <v>881</v>
+        <v>47</v>
       </c>
       <c r="B46" s="32" t="s">
-        <v>864</v>
+        <v>36</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="D46" s="32" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="32" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B47" s="32" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="32" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B48" s="32" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="32" t="s">
-        <v>62</v>
+        <v>877</v>
       </c>
       <c r="B49" s="32" t="s">
-        <v>58</v>
+        <v>873</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>56</v>
+        <v>865</v>
       </c>
       <c r="D49" s="32" t="s">
-        <v>28</v>
+        <v>861</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="32" t="s">
-        <v>63</v>
+        <v>878</v>
       </c>
       <c r="B50" s="32" t="s">
-        <v>59</v>
+        <v>873</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>57</v>
+        <v>866</v>
       </c>
       <c r="D50" s="32" t="s">
-        <v>28</v>
+        <v>861</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="32" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>865</v>
+        <v>873</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>54</v>
+        <v>867</v>
       </c>
       <c r="D51" s="32" t="s">
-        <v>28</v>
+        <v>861</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="32" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="B52" s="32" t="s">
-        <v>866</v>
+        <v>873</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>55</v>
+        <v>868</v>
       </c>
       <c r="D52" s="32" t="s">
-        <v>28</v>
+        <v>861</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="32" t="s">
-        <v>884</v>
+        <v>853</v>
       </c>
       <c r="B53" s="32" t="s">
-        <v>867</v>
+        <v>845</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>56</v>
+        <v>831</v>
       </c>
       <c r="D53" s="32" t="s">
-        <v>28</v>
+        <v>831</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B54" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D54" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="32" t="s">
+        <v>881</v>
+      </c>
+      <c r="B56" s="32" t="s">
+        <v>864</v>
+      </c>
+      <c r="C56" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B57" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C57" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D57" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B58" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C58" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D58" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C59" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C60" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D60" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="32" t="s">
+        <v>882</v>
+      </c>
+      <c r="B61" s="32" t="s">
+        <v>865</v>
+      </c>
+      <c r="C61" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D61" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="32" t="s">
+        <v>883</v>
+      </c>
+      <c r="B62" s="32" t="s">
+        <v>866</v>
+      </c>
+      <c r="C62" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D62" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="32" t="s">
+        <v>884</v>
+      </c>
+      <c r="B63" s="32" t="s">
+        <v>867</v>
+      </c>
+      <c r="C63" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D63" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="32" t="s">
         <v>885</v>
       </c>
-      <c r="B54" s="32" t="s">
+      <c r="B64" s="32" t="s">
         <v>868</v>
       </c>
-      <c r="C54" s="32" t="s">
+      <c r="C64" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="D54" s="32" t="s">
+      <c r="D64" s="32" t="s">
         <v>28</v>
       </c>
     </row>
@@ -15682,10 +15861,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15697,7 +15876,7 @@
     <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -15713,8 +15892,17 @@
       <c r="E1" t="s">
         <v>825</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>906</v>
+      </c>
+      <c r="G1" t="s">
+        <v>907</v>
+      </c>
+      <c r="H1" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>96</v>
       </c>
@@ -15729,6 +15917,15 @@
       </c>
       <c r="E2">
         <v>400</v>
+      </c>
+      <c r="F2">
+        <v>1E-4</v>
+      </c>
+      <c r="G2">
+        <v>500</v>
+      </c>
+      <c r="H2">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>